<commit_message>
Profile Picture Upload for ESS Users
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Batch20Group6.xlsx
+++ b/src/test/resources/testdata/Batch20Group6.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MARINA\SDET\GroupProject\Marina\Group6B20\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MARINA\SDET\GroupProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DDE7E3-D8DE-41A5-98E1-15BC20DA985A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92990A04-3095-4826-A1CB-D841ED75938E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2DA10F56-E53D-4ABA-9FBF-FFFB5FD6FBE2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Isabella</t>
   </si>
@@ -58,6 +58,24 @@
   </si>
   <si>
     <t>Profile Photo</t>
+  </si>
+  <si>
+    <t>Exceeded 1MB</t>
+  </si>
+  <si>
+    <t>Incorrect Dimensions</t>
+  </si>
+  <si>
+    <t>Unsupported File Format</t>
+  </si>
+  <si>
+    <t>D:\MARINA\SDET\GroupProject\Exceeded 1MB.jpg</t>
+  </si>
+  <si>
+    <t>D:\MARINA\SDET\GroupProject\Incorrect Dimensions.jpg</t>
+  </si>
+  <si>
+    <t>D:\MARINA\SDET\GroupProject\Unsupported FIle Format.bmp</t>
   </si>
 </sst>
 </file>
@@ -441,19 +459,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D735EE5-45D8-4AAD-B26D-60A15A553937}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="16.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.26953125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="13" style="1" customWidth="1"/>
+    <col min="4" max="4" width="52.90625" style="1" customWidth="1"/>
+    <col min="5" max="7" width="52.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -466,8 +485,17 @@
       <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -479,6 +507,15 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>